<commit_message>
updated agile methodology for schedule management
</commit_message>
<xml_diff>
--- a/Schedule Management.xlsx
+++ b/Schedule Management.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538362\Desktop\GDP-1-44691-01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538362\Desktop\GDP-1-44691-01\Health app\HealthApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF744DCC-6A03-4C55-9EE1-C014C5CF5F62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E142F9AC-032B-4AD5-8DCF-150CAAB0BB63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Start Date</t>
   </si>
@@ -117,13 +118,76 @@
   </si>
   <si>
     <t xml:space="preserve">   1.4.4 iOS App development</t>
+  </si>
+  <si>
+    <t>1.1 User Stories</t>
+  </si>
+  <si>
+    <t>1.3 Cost Estimation</t>
+  </si>
+  <si>
+    <t>1.4 Proposed Screens</t>
+  </si>
+  <si>
+    <t>1.5 Schedule Management</t>
+  </si>
+  <si>
+    <t>Sprint 1 - RFP</t>
+  </si>
+  <si>
+    <t>Sprint 2 - User Development</t>
+  </si>
+  <si>
+    <t>2.1 User UI development</t>
+  </si>
+  <si>
+    <t>2.2 User Database Design</t>
+  </si>
+  <si>
+    <t>2.3 User Implementation</t>
+  </si>
+  <si>
+    <t>2.4 User Deploy</t>
+  </si>
+  <si>
+    <t>1.3 ER Diagram</t>
+  </si>
+  <si>
+    <t>Sprint 3 - Admin Development</t>
+  </si>
+  <si>
+    <t>3.1 Admin UI development</t>
+  </si>
+  <si>
+    <t>3.2 Admin Database Design</t>
+  </si>
+  <si>
+    <t>3.3 Admin Implementation</t>
+  </si>
+  <si>
+    <t>3.4 Admin Deploy</t>
+  </si>
+  <si>
+    <t>Sprint 4 - Admin web Develop</t>
+  </si>
+  <si>
+    <t>4.1 Admin webpage UI</t>
+  </si>
+  <si>
+    <t>4.2 Admin BackEnd</t>
+  </si>
+  <si>
+    <t>4.3 Admin Implementation</t>
+  </si>
+  <si>
+    <t>4.4 Admin Deploy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +234,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,7 +255,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -202,11 +278,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -218,6 +314,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -502,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548BF8C0-CDAD-4580-B42C-05D6E3D594DB}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,4 +1143,572 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F33B4DB-8523-4C81-A3EF-A95BD919BE6D}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8">
+        <f>SUM(G5:G9)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <f>SUM(B5:F5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" ref="G6:G17" si="0">SUM(B6:F6)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
+        <f>SUM(B8:F8)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>2</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8">
+        <f>SUM(G11:G14)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="8">
+        <v>5</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>3</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>2</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <v>4</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8">
+        <v>2</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
+        <f>SUM(G16:G19)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8">
+        <v>3</v>
+      </c>
+      <c r="E16" s="8">
+        <v>5</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
+        <v>3</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2</v>
+      </c>
+      <c r="G17" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="8">
+        <v>3</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8">
+        <f>SUM(B18:F18)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
+        <v>4</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8">
+        <f>SUM(B19:F19)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8">
+        <f>SUM(G21:G24)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
+        <v>2</v>
+      </c>
+      <c r="G21" s="8">
+        <f>SUM(B21:F21)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8">
+        <v>3</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8">
+        <f t="shared" ref="G20:G24" si="1">SUM(B22:F22)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>2</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8">
+        <v>2</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8">
+        <v>3</v>
+      </c>
+      <c r="E24" s="8">
+        <v>2</v>
+      </c>
+      <c r="F24" s="8">
+        <v>3</v>
+      </c>
+      <c r="G24" s="8">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="7">
+        <f>SUM(B5:B24)</f>
+        <v>23</v>
+      </c>
+      <c r="C26" s="7">
+        <f>SUM(C5:C24)</f>
+        <v>18</v>
+      </c>
+      <c r="D26" s="7">
+        <f>SUM(D5:D24)</f>
+        <v>31</v>
+      </c>
+      <c r="E26" s="7">
+        <f>SUM(E5:E24)</f>
+        <v>33</v>
+      </c>
+      <c r="F26" s="7">
+        <f>SUM(F5:F24)</f>
+        <v>25</v>
+      </c>
+      <c r="G26" s="7">
+        <f>SUM(G4,G10,G15,G20)</f>
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>